<commit_message>
output file recreated, run.sh added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\github_repos\work-10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="244" yWindow="11" windowWidth="16095" windowHeight="9659"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -162,8 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,14 +221,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -280,7 +267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,10 +299,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,7 +333,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -523,20 +508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.09765625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -570,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -587,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -604,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -621,7 +600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -638,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -655,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -672,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -689,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -706,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -723,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -740,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -757,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -774,7 +753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -791,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -808,7 +787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -825,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -842,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -859,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -876,7 +855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -893,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -910,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -927,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>17</v>
       </c>

</xml_diff>